<commit_message>
Data Downloads, Webpage Selection
Additional job data added, website template added
</commit_message>
<xml_diff>
--- a/Data/Job_Titles.xlsx
+++ b/Data/Job_Titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariko\Documents\GitHub\Remote_Careers-DATS6401\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC5EB38-FDC3-431C-BF95-3E06206D9D1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCE5108-1A58-45EB-84AF-198A47C17A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CFCFF21E-6815-4865-9DE0-0DADF51387DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CFCFF21E-6815-4865-9DE0-0DADF51387DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Largest_cities" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3002" uniqueCount="2743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3114" uniqueCount="2849">
   <si>
     <t>11-3111</t>
   </si>
@@ -8355,22 +8355,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Charlotte Amalie</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color rgb="FF0645AD"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -8396,6 +8380,339 @@
   </si>
   <si>
     <t>Portland+ME</t>
+  </si>
+  <si>
+    <t>Second Most</t>
+  </si>
+  <si>
+    <t>Huntsville</t>
+  </si>
+  <si>
+    <t>Montgomery</t>
+  </si>
+  <si>
+    <t>Juneau</t>
+  </si>
+  <si>
+    <t>Fairbanks</t>
+  </si>
+  <si>
+    <t>Nu'uuli</t>
+  </si>
+  <si>
+    <t>Pago Pago</t>
+  </si>
+  <si>
+    <t>Tucson</t>
+  </si>
+  <si>
+    <t>Mesa</t>
+  </si>
+  <si>
+    <t>Fort Smith</t>
+  </si>
+  <si>
+    <t>Fayetteville</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>San Jose</t>
+  </si>
+  <si>
+    <t>Colorado Springs</t>
+  </si>
+  <si>
+    <t>Aurora</t>
+  </si>
+  <si>
+    <t>New Haven</t>
+  </si>
+  <si>
+    <t>Stamford</t>
+  </si>
+  <si>
+    <t>Dover</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Tampa</t>
+  </si>
+  <si>
+    <t>Augusta</t>
+  </si>
+  <si>
+    <t>Yigo</t>
+  </si>
+  <si>
+    <t>Tamuning</t>
+  </si>
+  <si>
+    <t>Meridian</t>
+  </si>
+  <si>
+    <t>Nampa</t>
+  </si>
+  <si>
+    <t>Naperville</t>
+  </si>
+  <si>
+    <t>Fort Wayne</t>
+  </si>
+  <si>
+    <t>Evansville</t>
+  </si>
+  <si>
+    <t>Cedar Rapids</t>
+  </si>
+  <si>
+    <t>Davenport</t>
+  </si>
+  <si>
+    <t>Overland Park</t>
+  </si>
+  <si>
+    <t>Lexington</t>
+  </si>
+  <si>
+    <t>Bowling Green</t>
+  </si>
+  <si>
+    <t>Shreveport</t>
+  </si>
+  <si>
+    <t>Lewiston</t>
+  </si>
+  <si>
+    <t>Bangor</t>
+  </si>
+  <si>
+    <t>Frederick</t>
+  </si>
+  <si>
+    <t>Rockville</t>
+  </si>
+  <si>
+    <t>Worcester</t>
+  </si>
+  <si>
+    <t>Springfield</t>
+  </si>
+  <si>
+    <t>Grand Rapids</t>
+  </si>
+  <si>
+    <t>Warren</t>
+  </si>
+  <si>
+    <t>Saint Paul</t>
+  </si>
+  <si>
+    <t>Rochester</t>
+  </si>
+  <si>
+    <t>Gulfport</t>
+  </si>
+  <si>
+    <t>Southaven</t>
+  </si>
+  <si>
+    <t>Saint Louis</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Missoula</t>
+  </si>
+  <si>
+    <t>Great Falls</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>Bellevue</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>Reno</t>
+  </si>
+  <si>
+    <t>Nashua</t>
+  </si>
+  <si>
+    <t>Concord</t>
+  </si>
+  <si>
+    <t>Jersey City</t>
+  </si>
+  <si>
+    <t>Paterson</t>
+  </si>
+  <si>
+    <t>Las Cruces</t>
+  </si>
+  <si>
+    <t>Rio Rancho</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Raleigh</t>
+  </si>
+  <si>
+    <t>Greensboro</t>
+  </si>
+  <si>
+    <t>Bismarck</t>
+  </si>
+  <si>
+    <t>Grand Forks</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>Tulsa</t>
+  </si>
+  <si>
+    <t>Norman</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>Eugene</t>
+  </si>
+  <si>
+    <t>Pittsburgh</t>
+  </si>
+  <si>
+    <t>Allentown</t>
+  </si>
+  <si>
+    <t>Bayamón</t>
+  </si>
+  <si>
+    <t>Carolina</t>
+  </si>
+  <si>
+    <t>Cranston</t>
+  </si>
+  <si>
+    <t>Warwick</t>
+  </si>
+  <si>
+    <t>North Charleston</t>
+  </si>
+  <si>
+    <t>Rapid City</t>
+  </si>
+  <si>
+    <t>Aberdeen</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Knoxville</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>West Valley City</t>
+  </si>
+  <si>
+    <t>Provo</t>
+  </si>
+  <si>
+    <t>South Burlington</t>
+  </si>
+  <si>
+    <t>Rutland</t>
+  </si>
+  <si>
+    <t>Norfolk</t>
+  </si>
+  <si>
+    <t>Chesapeake</t>
+  </si>
+  <si>
+    <t>Spokane</t>
+  </si>
+  <si>
+    <t>Tacoma</t>
+  </si>
+  <si>
+    <t>Huntington</t>
+  </si>
+  <si>
+    <t>Morgantown</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>Green Bay</t>
+  </si>
+  <si>
+    <t>Casper</t>
+  </si>
+  <si>
+    <t>Laramie</t>
+  </si>
+  <si>
+    <t>Third Most</t>
+  </si>
+  <si>
+    <t>Pearl City</t>
+  </si>
+  <si>
+    <r>
+      <t>East Honolulu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202122"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Baton Rouge</t>
+  </si>
+  <si>
+    <t>Rota</t>
+  </si>
+  <si>
+    <t>Tinian</t>
+  </si>
+  <si>
+    <t>Charlotte Amalie</t>
+  </si>
+  <si>
+    <t>Sion Farm</t>
+  </si>
+  <si>
+    <t>Northside</t>
   </si>
 </sst>
 </file>
@@ -8557,7 +8874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -8598,12 +8915,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -8620,6 +8931,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -15776,472 +16099,812 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6CE42B-7840-40D4-8D0E-7CFC8CB55E6A}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.85546875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>2737</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>2740</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>2742</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>2630</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>2631</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>2743</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>2744</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>2632</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>2633</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>2745</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>2746</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>2634</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>2635</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>2747</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>2748</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>2636</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>2637</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2749</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>2638</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>2639</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>2751</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>2752</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>2640</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>2641</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>2753</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>2643</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>2755</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>2644</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>2645</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>2757</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>2758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>2646</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>2647</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>2759</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>2648</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>2649</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>2650</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>2651</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>2652</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>2760</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>2761</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>2653</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>2654</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>2762</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>2655</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>2656</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>2657</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>2763</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>2764</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>2658</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>2739</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>2842</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>2841</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>2659</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>2660</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>2765</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>2766</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>2662</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>2756</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>2767</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>2663</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>2768</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>2769</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>2665</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>2666</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>2770</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>2771</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>2667</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>2668</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>2772</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>2670</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>2671</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>2773</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>2774</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>2673</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>2843</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>2775</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>2674</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>2741</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>2776</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
         <v>2738</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>2741</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>2630</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>2631</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>2632</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>2633</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>2634</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>2635</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>2636</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>2637</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>2638</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>2639</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>2640</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>2641</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>2642</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>2643</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>2644</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>2645</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>2646</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>2647</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>2649</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>2650</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>2651</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>2652</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>2653</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>2654</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>2656</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>2657</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>2658</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>2740</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>2659</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>2660</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>2661</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>2662</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>2663</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>2664</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>2665</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>2666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>2667</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>2668</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
-        <v>2670</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>2671</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>2672</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>2673</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>2674</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>2742</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
-        <v>2739</v>
-      </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="14" t="s">
         <v>2676</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+      <c r="C24" s="14" t="s">
+        <v>2778</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>2779</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
         <v>2677</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="15" t="s">
         <v>2678</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
+      <c r="C25" s="14" t="s">
+        <v>2780</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
         <v>2679</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="14" t="s">
         <v>2680</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="C26" s="14" t="s">
+        <v>2782</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
         <v>2681</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="14" t="s">
         <v>2682</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="C27" s="15" t="s">
+        <v>2784</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>2785</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
         <v>2683</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="15" t="s">
         <v>2684</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+      <c r="C28" s="14" t="s">
+        <v>2786</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>2787</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
         <v>2685</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="14" t="s">
         <v>2669</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+      <c r="C29" s="14" t="s">
+        <v>2788</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>2781</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
         <v>2686</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="14" t="s">
         <v>2687</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+      <c r="C30" s="14" t="s">
+        <v>2790</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>2791</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
         <v>2688</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>2689</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="C31" s="15" t="s">
+        <v>2792</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
         <v>2690</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="14" t="s">
         <v>2691</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+      <c r="C32" s="14" t="s">
+        <v>2794</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>2795</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
         <v>2692</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>2693</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
+      <c r="C33" s="14" t="s">
+        <v>2796</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>2694</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="14" t="s">
         <v>2648</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+      <c r="C34" s="14" t="s">
+        <v>2798</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
         <v>2695</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="14" t="s">
         <v>2696</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
+      <c r="C35" s="14" t="s">
+        <v>2800</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>2801</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
         <v>2697</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="14" t="s">
         <v>2698</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+      <c r="C36" s="14" t="s">
+        <v>2802</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>2785</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
         <v>2699</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="14" t="s">
         <v>2700</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
+      <c r="C37" s="15" t="s">
+        <v>2803</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>2804</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
         <v>2701</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="14" t="s">
         <v>2702</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
+      <c r="C38" s="15" t="s">
+        <v>2805</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>2806</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
         <v>2703</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="18" t="s">
         <v>2735</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
+      <c r="C39" s="23" t="s">
+        <v>2845</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
         <v>2704</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="15" t="s">
         <v>2655</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+      <c r="C40" s="14" t="s">
+        <v>2807</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>2808</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
         <v>2705</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="15" t="s">
         <v>2706</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+      <c r="C41" s="14" t="s">
+        <v>2809</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>2810</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
         <v>2707</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="14" t="s">
         <v>2675</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+      <c r="C42" s="15" t="s">
+        <v>2811</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>2708</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="14" t="s">
         <v>2709</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
+      <c r="C43" s="14" t="s">
+        <v>2813</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>2814</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
         <v>2710</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="15" t="s">
         <v>2711</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
+      <c r="C44" s="14" t="s">
+        <v>2815</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>2816</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="14" t="s">
         <v>2712</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="15" t="s">
         <v>2713</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
+      <c r="C45" s="14" t="s">
+        <v>2817</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>2818</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
         <v>2714</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="14" t="s">
         <v>2715</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
+      <c r="C46" s="15" t="s">
+        <v>2789</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
         <v>2716</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="14" t="s">
         <v>2717</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="16" t="s">
+      <c r="C47" s="14" t="s">
+        <v>2820</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>2821</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="14" t="s">
         <v>2718</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="15" t="s">
         <v>2719</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="16" t="s">
+      <c r="C48" s="14" t="s">
+        <v>2822</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>2823</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
         <v>2720</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="14" t="s">
         <v>2721</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="16" t="s">
+      <c r="C49" s="14" t="s">
+        <v>2824</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>2825</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14" t="s">
         <v>2722</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="15" t="s">
         <v>2723</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
+      <c r="C50" s="14" t="s">
+        <v>2826</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>2827</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
         <v>2724</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="14" t="s">
         <v>2725</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
+      <c r="C51" s="14" t="s">
+        <v>2828</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>2829</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="17" t="s">
         <v>2736</v>
       </c>
-      <c r="B52" s="20" t="s">
-        <v>2737</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="16" t="s">
+      <c r="B52" s="18" t="s">
+        <v>2846</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>2847</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
         <v>2726</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="14" t="s">
         <v>2727</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="16" t="s">
+      <c r="C53" s="14" t="s">
+        <v>2830</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>2831</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="14" t="s">
         <v>2728</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="14" t="s">
         <v>2729</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16" t="s">
+      <c r="C54" s="14" t="s">
+        <v>2832</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="14" t="s">
         <v>2730</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="15" t="s">
         <v>2715</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16" t="s">
+      <c r="C55" s="14" t="s">
+        <v>2834</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>2835</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14" t="s">
         <v>2731</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="14" t="s">
         <v>2732</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
+      <c r="C56" s="15" t="s">
+        <v>2836</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>2837</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14" t="s">
         <v>2733</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="15" t="s">
         <v>2734</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>2838</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>2839</v>
       </c>
     </row>
   </sheetData>
@@ -16353,10 +17016,114 @@
     <hyperlink ref="B56" r:id="rId105" tooltip="Milwaukee" display="https://en.wikipedia.org/wiki/Milwaukee" xr:uid="{69F36A11-AE4D-4269-A718-B44BF2B7D236}"/>
     <hyperlink ref="A57" r:id="rId106" tooltip="Wyoming" display="https://en.wikipedia.org/wiki/Wyoming" xr:uid="{1FA5CB2A-77EA-4EC5-A04E-6B2EE99547A5}"/>
     <hyperlink ref="B57" r:id="rId107" tooltip="Cheyenne, Wyoming" display="https://en.wikipedia.org/wiki/Cheyenne,_Wyoming" xr:uid="{9FD2739C-844C-4FBF-8338-AEA262C586EC}"/>
+    <hyperlink ref="C2" r:id="rId108" tooltip="Huntsville, Alabama" display="https://en.wikipedia.org/wiki/Huntsville,_Alabama" xr:uid="{C6AD7134-0B30-4BA8-B3E5-C17DBC25B4D7}"/>
+    <hyperlink ref="C3" r:id="rId109" tooltip="Juneau, Alaska" display="https://en.wikipedia.org/wiki/Juneau,_Alaska" xr:uid="{44CF5F1F-32F8-4333-9BC3-A901BA359E1D}"/>
+    <hyperlink ref="C4" r:id="rId110" tooltip="Nu'uuli, American Samoa" display="https://en.wikipedia.org/wiki/Nu%27uuli,_American_Samoa" xr:uid="{E51A9503-3561-43CC-8C9A-AE700763C993}"/>
+    <hyperlink ref="C5" r:id="rId111" tooltip="Tucson, Arizona" display="https://en.wikipedia.org/wiki/Tucson,_Arizona" xr:uid="{677E5986-6DC8-476D-A39F-AFAF98AB5942}"/>
+    <hyperlink ref="C6" r:id="rId112" tooltip="Fort Smith, Arkansas" display="https://en.wikipedia.org/wiki/Fort_Smith,_Arkansas" xr:uid="{F219DC11-8559-48A1-8C4C-F3429CE9CB49}"/>
+    <hyperlink ref="C7" r:id="rId113" tooltip="San Diego" display="https://en.wikipedia.org/wiki/San_Diego" xr:uid="{5D40D81B-B07E-404E-8A02-56FD0A12C667}"/>
+    <hyperlink ref="C8" r:id="rId114" tooltip="Colorado Springs, Colorado" display="https://en.wikipedia.org/wiki/Colorado_Springs,_Colorado" xr:uid="{1A058DF3-1B74-4664-9D3A-E325654E48F7}"/>
+    <hyperlink ref="C9" r:id="rId115" tooltip="New Haven, Connecticut" display="https://en.wikipedia.org/wiki/New_Haven,_Connecticut" xr:uid="{00176A4E-35E7-4715-9821-1AA4BC66DB08}"/>
+    <hyperlink ref="C10" r:id="rId116" tooltip="Dover, Delaware" display="https://en.wikipedia.org/wiki/Dover,_Delaware" xr:uid="{B426002B-42E5-4A94-B892-0BF373D5EB60}"/>
+    <hyperlink ref="C12" r:id="rId117" tooltip="Miami, Florida" display="https://en.wikipedia.org/wiki/Miami,_Florida" xr:uid="{6FFD6267-D628-4560-B297-EA0275F95F53}"/>
+    <hyperlink ref="C13" r:id="rId118" tooltip="Augusta, Georgia" display="https://en.wikipedia.org/wiki/Augusta,_Georgia" xr:uid="{3DA2F7E1-3592-4AAD-8F8C-01B921ED17CC}"/>
+    <hyperlink ref="C14" r:id="rId119" tooltip="Yigo, Guam" display="https://en.wikipedia.org/wiki/Yigo,_Guam" xr:uid="{BE0BD581-D430-4FDD-B44F-80257DCE98B1}"/>
+    <hyperlink ref="C16" r:id="rId120" tooltip="Meridian, Idaho" display="https://en.wikipedia.org/wiki/Meridian,_Idaho" xr:uid="{E04F729C-9E73-4F8D-A7A5-AC588420F16C}"/>
+    <hyperlink ref="C17" r:id="rId121" tooltip="Aurora, Illinois" display="https://en.wikipedia.org/wiki/Aurora,_Illinois" xr:uid="{8C780644-B4B5-4668-A8A7-533907076A0F}"/>
+    <hyperlink ref="C18" r:id="rId122" tooltip="Fort Wayne, Indiana" display="https://en.wikipedia.org/wiki/Fort_Wayne,_Indiana" xr:uid="{98AE6859-88DE-40C8-B590-4A01FBF734E2}"/>
+    <hyperlink ref="C19" r:id="rId123" tooltip="Cedar Rapids, Iowa" display="https://en.wikipedia.org/wiki/Cedar_Rapids,_Iowa" xr:uid="{45BAF012-5815-4512-8786-78F4A09F487D}"/>
+    <hyperlink ref="C20" r:id="rId124" tooltip="Overland Park, Kansas" display="https://en.wikipedia.org/wiki/Overland_Park,_Kansas" xr:uid="{5336DCEF-F870-48EC-A30D-0455B0D756C7}"/>
+    <hyperlink ref="C21" r:id="rId125" tooltip="Lexington, Kentucky" display="https://en.wikipedia.org/wiki/Lexington,_Kentucky" xr:uid="{454F2D09-5A8A-4852-8342-19AD7096D6D8}"/>
+    <hyperlink ref="C22" r:id="rId126" tooltip="Baton Rouge" display="https://en.wikipedia.org/wiki/Baton_Rouge" xr:uid="{9C63B8F2-789F-49A0-8D59-0CD0B3C2BBD3}"/>
+    <hyperlink ref="C23" r:id="rId127" tooltip="Lewiston, Maine" display="https://en.wikipedia.org/wiki/Lewiston,_Maine" xr:uid="{04A20E03-F34C-44D6-BBF6-003E041D4B58}"/>
+    <hyperlink ref="C24" r:id="rId128" tooltip="Frederick, Maryland" display="https://en.wikipedia.org/wiki/Frederick,_Maryland" xr:uid="{2167EE97-3C19-4037-8E2B-50D69BF29C0E}"/>
+    <hyperlink ref="C25" r:id="rId129" tooltip="Worcester, Massachusetts" display="https://en.wikipedia.org/wiki/Worcester,_Massachusetts" xr:uid="{60FFD18F-0200-432A-AD30-C098CFD07CB1}"/>
+    <hyperlink ref="C26" r:id="rId130" tooltip="Grand Rapids, Michigan" display="https://en.wikipedia.org/wiki/Grand_Rapids,_Michigan" xr:uid="{709D1A5F-436F-4173-96B7-26DC89BDDCB4}"/>
+    <hyperlink ref="C27" r:id="rId131" tooltip="St. Paul, Minnesota" display="https://en.wikipedia.org/wiki/St._Paul,_Minnesota" xr:uid="{AB2EE096-DB93-41F6-A726-6E89B146A598}"/>
+    <hyperlink ref="C28" r:id="rId132" tooltip="Gulfport, Mississippi" display="https://en.wikipedia.org/wiki/Gulfport,_Mississippi" xr:uid="{21E961B3-BDB1-4ECB-9774-D826BDDEB658}"/>
+    <hyperlink ref="C29" r:id="rId133" tooltip="St. Louis" display="https://en.wikipedia.org/wiki/St._Louis" xr:uid="{9FA0D1D1-0E61-41F7-92CC-073E27E6FAE8}"/>
+    <hyperlink ref="C30" r:id="rId134" tooltip="Missoula, Montana" display="https://en.wikipedia.org/wiki/Missoula,_Montana" xr:uid="{052C6B9C-2075-47AF-816A-0C3D969457CC}"/>
+    <hyperlink ref="C31" r:id="rId135" tooltip="Lincoln, Nebraska" display="https://en.wikipedia.org/wiki/Lincoln,_Nebraska" xr:uid="{222624DB-E1FF-4BF6-A78C-6273178C960B}"/>
+    <hyperlink ref="C32" r:id="rId136" tooltip="Henderson, Nevada" display="https://en.wikipedia.org/wiki/Henderson,_Nevada" xr:uid="{14D4D88C-4651-4EA2-8B19-DF183EEB57F0}"/>
+    <hyperlink ref="C33" r:id="rId137" tooltip="Nashua, New Hampshire" display="https://en.wikipedia.org/wiki/Nashua,_New_Hampshire" xr:uid="{D498CFF8-6F5F-4838-A181-4C091F94C98F}"/>
+    <hyperlink ref="C34" r:id="rId138" tooltip="Jersey City, New Jersey" display="https://en.wikipedia.org/wiki/Jersey_City,_New_Jersey" xr:uid="{767FF7EF-11A2-4698-920E-233436EB55DC}"/>
+    <hyperlink ref="C35" r:id="rId139" tooltip="Las Cruces, New Mexico" display="https://en.wikipedia.org/wiki/Las_Cruces,_New_Mexico" xr:uid="{ED9C1D65-C1F1-48FD-82EB-B9D76CFC5320}"/>
+    <hyperlink ref="C36" r:id="rId140" tooltip="Buffalo, New York" display="https://en.wikipedia.org/wiki/Buffalo,_New_York" xr:uid="{7632409C-33B8-4EF5-AC38-7F7CA0375809}"/>
+    <hyperlink ref="C37" r:id="rId141" tooltip="Raleigh, North Carolina" display="https://en.wikipedia.org/wiki/Raleigh,_North_Carolina" xr:uid="{BB36F8BB-183E-448F-8261-23DF7ED16E7E}"/>
+    <hyperlink ref="C38" r:id="rId142" tooltip="Bismarck, North Dakota" display="https://en.wikipedia.org/wiki/Bismarck,_North_Dakota" xr:uid="{DB16FF47-5241-4165-A4E6-3F89101E5880}"/>
+    <hyperlink ref="C40" r:id="rId143" tooltip="Cleveland" display="https://en.wikipedia.org/wiki/Cleveland" xr:uid="{321E24AA-DFDF-496C-9808-37BEEFD82F48}"/>
+    <hyperlink ref="C41" r:id="rId144" tooltip="Tulsa, Oklahoma" display="https://en.wikipedia.org/wiki/Tulsa,_Oklahoma" xr:uid="{1B5BAF75-BA93-41A0-8365-DF00EF478685}"/>
+    <hyperlink ref="C42" r:id="rId145" tooltip="Salem, Oregon" display="https://en.wikipedia.org/wiki/Salem,_Oregon" xr:uid="{EDFFFA08-6ACD-4FCA-BFBC-CDA021732C4D}"/>
+    <hyperlink ref="C43" r:id="rId146" tooltip="Pittsburgh" display="https://en.wikipedia.org/wiki/Pittsburgh" xr:uid="{65CFAFBA-016C-4318-904C-E97DB3356E3A}"/>
+    <hyperlink ref="C44" r:id="rId147" tooltip="Bayamón, Puerto Rico" display="https://en.wikipedia.org/wiki/Bayam%C3%B3n,_Puerto_Rico" xr:uid="{FF3F20C0-B00E-4298-BDA3-66B8E9F6B296}"/>
+    <hyperlink ref="C45" r:id="rId148" tooltip="Cranston, Rhode Island" display="https://en.wikipedia.org/wiki/Cranston,_Rhode_Island" xr:uid="{BB8094AE-AA76-4D1A-B5C2-AE76A495A449}"/>
+    <hyperlink ref="C46" r:id="rId149" tooltip="Columbia, South Carolina" display="https://en.wikipedia.org/wiki/Columbia,_South_Carolina" xr:uid="{EC89548A-3E48-4449-81D5-2400BC166470}"/>
+    <hyperlink ref="C47" r:id="rId150" tooltip="Rapid City, South Dakota" display="https://en.wikipedia.org/wiki/Rapid_City,_South_Dakota" xr:uid="{FD547F9B-C483-4B11-9FFD-28D47183BFF1}"/>
+    <hyperlink ref="C48" r:id="rId151" tooltip="Memphis, Tennessee" display="https://en.wikipedia.org/wiki/Memphis,_Tennessee" xr:uid="{A61338B1-D69E-401E-B67D-6A712BEC8F2E}"/>
+    <hyperlink ref="C49" r:id="rId152" tooltip="San Antonio" display="https://en.wikipedia.org/wiki/San_Antonio" xr:uid="{A7279B93-9962-4ED8-8CAA-086BE4E9DF18}"/>
+    <hyperlink ref="C50" r:id="rId153" tooltip="West Valley City, Utah" display="https://en.wikipedia.org/wiki/West_Valley_City,_Utah" xr:uid="{780B6214-1AB7-499E-98AE-0FF9246924A2}"/>
+    <hyperlink ref="C51" r:id="rId154" tooltip="South Burlington, Vermont" display="https://en.wikipedia.org/wiki/South_Burlington,_Vermont" xr:uid="{99168789-AFA0-4DC4-853D-54EEFE95FD6E}"/>
+    <hyperlink ref="C53" r:id="rId155" tooltip="Norfolk, Virginia" display="https://en.wikipedia.org/wiki/Norfolk,_Virginia" xr:uid="{9B1356E0-2234-41EC-8038-8AB40132E296}"/>
+    <hyperlink ref="C54" r:id="rId156" tooltip="Spokane, Washington" display="https://en.wikipedia.org/wiki/Spokane,_Washington" xr:uid="{AF75FE47-3401-4A20-91BC-3CB76F27A77C}"/>
+    <hyperlink ref="C55" r:id="rId157" tooltip="Huntington, West Virginia" display="https://en.wikipedia.org/wiki/Huntington,_West_Virginia" xr:uid="{5779BF10-2ABC-461B-8D00-95CA5F8637BE}"/>
+    <hyperlink ref="C56" r:id="rId158" tooltip="Madison, Wisconsin" display="https://en.wikipedia.org/wiki/Madison,_Wisconsin" xr:uid="{CED4466C-2B68-4B73-9729-7B219819CBD6}"/>
+    <hyperlink ref="C57" r:id="rId159" tooltip="Casper, Wyoming" display="https://en.wikipedia.org/wiki/Casper,_Wyoming" xr:uid="{98CDBD7D-BEA9-4B13-B38D-A4A880F149A9}"/>
+    <hyperlink ref="D2" r:id="rId160" tooltip="Montgomery, Alabama" display="https://en.wikipedia.org/wiki/Montgomery,_Alabama" xr:uid="{781684F8-A260-4A6F-A937-6236F294B295}"/>
+    <hyperlink ref="D3" r:id="rId161" tooltip="Fairbanks, Alaska" display="https://en.wikipedia.org/wiki/Fairbanks,_Alaska" xr:uid="{E1092C2A-0DE9-43A8-A631-3F4E66CCFE13}"/>
+    <hyperlink ref="D4" r:id="rId162" tooltip="Pago Pago" display="https://en.wikipedia.org/wiki/Pago_Pago" xr:uid="{D61B64D3-A8FD-452D-9D0D-02B990F831BE}"/>
+    <hyperlink ref="D5" r:id="rId163" tooltip="Mesa, Arizona" display="https://en.wikipedia.org/wiki/Mesa,_Arizona" xr:uid="{36B5B864-C418-4A55-A9A8-3C0E06CD745E}"/>
+    <hyperlink ref="D6" r:id="rId164" tooltip="Fayetteville, Arkansas" display="https://en.wikipedia.org/wiki/Fayetteville,_Arkansas" xr:uid="{07115E13-FCB0-4D7F-95C4-AD7685DC72A8}"/>
+    <hyperlink ref="D7" r:id="rId165" tooltip="San Jose, California" display="https://en.wikipedia.org/wiki/San_Jose,_California" xr:uid="{8D97D820-C2F7-4D47-8540-74D7F28A0975}"/>
+    <hyperlink ref="D8" r:id="rId166" tooltip="Aurora, Colorado" display="https://en.wikipedia.org/wiki/Aurora,_Colorado" xr:uid="{E447F518-6123-4737-BD6B-B0CD9E2E16C5}"/>
+    <hyperlink ref="D9" r:id="rId167" tooltip="Stamford, Connecticut" display="https://en.wikipedia.org/wiki/Stamford,_Connecticut" xr:uid="{6CA7603F-55B9-4C70-B708-D0B3BDF01F0F}"/>
+    <hyperlink ref="D10" r:id="rId168" tooltip="Newark, Delaware" display="https://en.wikipedia.org/wiki/Newark,_Delaware" xr:uid="{015C9C2F-CD20-4F9B-BBEF-541A9EB79498}"/>
+    <hyperlink ref="D12" r:id="rId169" tooltip="Tampa, Florida" display="https://en.wikipedia.org/wiki/Tampa,_Florida" xr:uid="{2D086EEB-39D4-4432-B4F7-1BCA889D93F1}"/>
+    <hyperlink ref="D13" r:id="rId170" tooltip="Columbus, Georgia" display="https://en.wikipedia.org/wiki/Columbus,_Georgia" xr:uid="{688CA59F-EF1B-45B3-9E4B-BA84E329C06E}"/>
+    <hyperlink ref="D14" r:id="rId171" tooltip="Tamuning, Guam" display="https://en.wikipedia.org/wiki/Tamuning,_Guam" xr:uid="{A0965D1B-1680-4D68-867F-899ECB8A6403}"/>
+    <hyperlink ref="D16" r:id="rId172" tooltip="Nampa, Idaho" display="https://en.wikipedia.org/wiki/Nampa,_Idaho" xr:uid="{1FE2C505-6587-4183-8D49-2815F6C382C1}"/>
+    <hyperlink ref="D17" r:id="rId173" tooltip="Naperville, Illinois" display="https://en.wikipedia.org/wiki/Naperville,_Illinois" xr:uid="{D39FCBB4-F670-4A09-8471-FD88DC9FCD49}"/>
+    <hyperlink ref="D18" r:id="rId174" tooltip="Evansville, Indiana" display="https://en.wikipedia.org/wiki/Evansville,_Indiana" xr:uid="{421F09B0-C9A5-496E-B6AC-4566025B9089}"/>
+    <hyperlink ref="D19" r:id="rId175" tooltip="Davenport, Iowa" display="https://en.wikipedia.org/wiki/Davenport,_Iowa" xr:uid="{645DB8AC-5305-4607-86A0-A1443ACB361C}"/>
+    <hyperlink ref="D20" r:id="rId176" tooltip="Kansas City, Kansas" display="https://en.wikipedia.org/wiki/Kansas_City,_Kansas" xr:uid="{790829CB-7A6D-4C8D-BD17-634C898DD077}"/>
+    <hyperlink ref="D21" r:id="rId177" tooltip="Bowling Green, Kentucky" display="https://en.wikipedia.org/wiki/Bowling_Green,_Kentucky" xr:uid="{9E5F8E98-C69F-41E6-BEB4-B6F0EE14D6A7}"/>
+    <hyperlink ref="D22" r:id="rId178" tooltip="Shreveport, Louisiana" display="https://en.wikipedia.org/wiki/Shreveport,_Louisiana" xr:uid="{F936FE48-1BC6-4EF4-9931-12224631DA43}"/>
+    <hyperlink ref="D23" r:id="rId179" tooltip="Bangor, Maine" display="https://en.wikipedia.org/wiki/Bangor,_Maine" xr:uid="{AABD179F-5727-4F0B-8618-841993559ECC}"/>
+    <hyperlink ref="D24" r:id="rId180" tooltip="Rockville, Maryland" display="https://en.wikipedia.org/wiki/Rockville,_Maryland" xr:uid="{91478AAB-BE06-44D2-93C4-DCC92E5FB929}"/>
+    <hyperlink ref="D25" r:id="rId181" tooltip="Springfield, Massachusetts" display="https://en.wikipedia.org/wiki/Springfield,_Massachusetts" xr:uid="{8B8CA66A-B011-4CC5-A262-F618118CE209}"/>
+    <hyperlink ref="D26" r:id="rId182" tooltip="Warren, Michigan" display="https://en.wikipedia.org/wiki/Warren,_Michigan" xr:uid="{63B23625-2C2E-4AAA-B44D-BD20E11A712E}"/>
+    <hyperlink ref="D27" r:id="rId183" tooltip="Rochester, Minnesota" display="https://en.wikipedia.org/wiki/Rochester,_Minnesota" xr:uid="{DA1BA257-812F-4E1E-8668-23EE16B8797A}"/>
+    <hyperlink ref="D28" r:id="rId184" tooltip="Southaven, Mississippi" display="https://en.wikipedia.org/wiki/Southaven,_Mississippi" xr:uid="{6B59D3AF-24F7-442E-9936-9F927946DEB4}"/>
+    <hyperlink ref="D29" r:id="rId185" tooltip="Springfield, Missouri" display="https://en.wikipedia.org/wiki/Springfield,_Missouri" xr:uid="{07D9B286-764C-4599-A4B9-44195B52DEC5}"/>
+    <hyperlink ref="D30" r:id="rId186" tooltip="Great Falls, Montana" display="https://en.wikipedia.org/wiki/Great_Falls,_Montana" xr:uid="{BCC6ACBB-C723-4A8D-96B6-3D8241A1405A}"/>
+    <hyperlink ref="D31" r:id="rId187" tooltip="Bellevue, Nebraska" display="https://en.wikipedia.org/wiki/Bellevue,_Nebraska" xr:uid="{7E36A179-A762-453E-854C-988F9DB823A6}"/>
+    <hyperlink ref="D32" r:id="rId188" tooltip="Reno, Nevada" display="https://en.wikipedia.org/wiki/Reno,_Nevada" xr:uid="{F6CF8AC0-4B3E-4CF3-951A-48825DD09972}"/>
+    <hyperlink ref="D33" r:id="rId189" tooltip="Concord, New Hampshire" display="https://en.wikipedia.org/wiki/Concord,_New_Hampshire" xr:uid="{CDF5FEFD-418E-4F17-9907-EDE767C36D62}"/>
+    <hyperlink ref="D34" r:id="rId190" tooltip="Paterson, New Jersey" display="https://en.wikipedia.org/wiki/Paterson,_New_Jersey" xr:uid="{0647A8AA-E745-4A62-BEA0-93133BA6F9FA}"/>
+    <hyperlink ref="D35" r:id="rId191" tooltip="Rio Rancho" display="https://en.wikipedia.org/wiki/Rio_Rancho" xr:uid="{173E5625-47C5-42DC-9C72-40FF3BC3F225}"/>
+    <hyperlink ref="D36" r:id="rId192" tooltip="Rochester, New York" display="https://en.wikipedia.org/wiki/Rochester,_New_York" xr:uid="{014BE270-1860-4907-9369-9C29A4F40B63}"/>
+    <hyperlink ref="D37" r:id="rId193" tooltip="Greensboro, North Carolina" display="https://en.wikipedia.org/wiki/Greensboro,_North_Carolina" xr:uid="{6422B0F0-7A12-4377-8CF9-6D21EEB9484F}"/>
+    <hyperlink ref="D38" r:id="rId194" tooltip="Grand Forks, North Dakota" display="https://en.wikipedia.org/wiki/Grand_Forks,_North_Dakota" xr:uid="{C9F90DA5-F36E-4839-A07B-9748CE628A95}"/>
+    <hyperlink ref="D40" r:id="rId195" tooltip="Cincinnati" display="https://en.wikipedia.org/wiki/Cincinnati" xr:uid="{0E7FB30F-8F59-4891-A21C-AF0271EAC317}"/>
+    <hyperlink ref="D41" r:id="rId196" tooltip="Norman, Oklahoma" display="https://en.wikipedia.org/wiki/Norman,_Oklahoma" xr:uid="{7311C658-F86F-4F18-8C7A-16CE881E0F5F}"/>
+    <hyperlink ref="D42" r:id="rId197" tooltip="Eugene, Oregon" display="https://en.wikipedia.org/wiki/Eugene,_Oregon" xr:uid="{75FD548A-1DA3-442B-AB0D-1356CAA05180}"/>
+    <hyperlink ref="D43" r:id="rId198" tooltip="Allentown, Pennsylvania" display="https://en.wikipedia.org/wiki/Allentown,_Pennsylvania" xr:uid="{5E6D1A6E-2C87-4B3F-BFDA-D7329EE7F3F8}"/>
+    <hyperlink ref="D44" r:id="rId199" tooltip="Carolina, Puerto Rico" display="https://en.wikipedia.org/wiki/Carolina,_Puerto_Rico" xr:uid="{AB0F38D1-84E2-43A6-A376-FAE7BF66315D}"/>
+    <hyperlink ref="D45" r:id="rId200" tooltip="Warwick, Rhode Island" display="https://en.wikipedia.org/wiki/Warwick,_Rhode_Island" xr:uid="{267D6C7A-1764-4814-8C7E-F4C56C7AE53C}"/>
+    <hyperlink ref="D46" r:id="rId201" tooltip="North Charleston, South Carolina" display="https://en.wikipedia.org/wiki/North_Charleston,_South_Carolina" xr:uid="{5DD42E50-80EE-440D-BB5A-6AC1A30F0776}"/>
+    <hyperlink ref="D47" r:id="rId202" tooltip="Aberdeen, South Dakota" display="https://en.wikipedia.org/wiki/Aberdeen,_South_Dakota" xr:uid="{9C4EF233-A524-4E64-BEF8-361AE553069A}"/>
+    <hyperlink ref="D48" r:id="rId203" tooltip="Knoxville, Tennessee" display="https://en.wikipedia.org/wiki/Knoxville,_Tennessee" xr:uid="{7543B54A-753D-42E1-901D-C85021763DD8}"/>
+    <hyperlink ref="D49" r:id="rId204" tooltip="Dallas" display="https://en.wikipedia.org/wiki/Dallas" xr:uid="{D1888D95-D57E-4803-B6F2-E3CDE979D19B}"/>
+    <hyperlink ref="D50" r:id="rId205" tooltip="Provo, Utah" display="https://en.wikipedia.org/wiki/Provo,_Utah" xr:uid="{58EC19E7-9A7F-49B9-9010-EDB820F335F9}"/>
+    <hyperlink ref="D51" r:id="rId206" tooltip="Rutland (city), Vermont" display="https://en.wikipedia.org/wiki/Rutland_(city),_Vermont" xr:uid="{94A19348-F6A8-43AD-99EC-B9E5439367FC}"/>
+    <hyperlink ref="D53" r:id="rId207" tooltip="Chesapeake, Virginia" display="https://en.wikipedia.org/wiki/Chesapeake,_Virginia" xr:uid="{209B98C4-25CC-4D25-82E1-833A63ACB369}"/>
+    <hyperlink ref="D54" r:id="rId208" tooltip="Tacoma, Washington" display="https://en.wikipedia.org/wiki/Tacoma,_Washington" xr:uid="{86AEB543-5AD6-438B-9578-0B6FE038EDEE}"/>
+    <hyperlink ref="D55" r:id="rId209" tooltip="Morgantown, West Virginia" display="https://en.wikipedia.org/wiki/Morgantown,_West_Virginia" xr:uid="{25D28A70-D555-42EF-96FA-7D3010948166}"/>
+    <hyperlink ref="D56" r:id="rId210" tooltip="Green Bay, Wisconsin" display="https://en.wikipedia.org/wiki/Green_Bay,_Wisconsin" xr:uid="{369471A3-E7C1-4834-923B-F30A7766EA0B}"/>
+    <hyperlink ref="D57" r:id="rId211" tooltip="Laramie, Wyoming" display="https://en.wikipedia.org/wiki/Laramie,_Wyoming" xr:uid="{DBC39B16-637C-40BF-B9DE-3D5696F46AD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId108"/>
-  <drawing r:id="rId109"/>
+  <pageSetup orientation="portrait" r:id="rId212"/>
+  <drawing r:id="rId213"/>
 </worksheet>
 </file>
 
@@ -16364,7 +17131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B93C22F-D58D-40FA-B35F-3AED71191FCA}">
   <dimension ref="A1:E1483"/>
   <sheetViews>
-    <sheetView topLeftCell="A346" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A346" workbookViewId="0">
       <selection activeCell="E350" sqref="E350"/>
     </sheetView>
   </sheetViews>
@@ -28943,9 +29710,9 @@
       </c>
     </row>
     <row r="1229" spans="1:4" ht="153" x14ac:dyDescent="0.25">
-      <c r="A1229" s="14"/>
-      <c r="B1229" s="14"/>
-      <c r="C1229" s="15" t="s">
+      <c r="A1229" s="20"/>
+      <c r="B1229" s="20"/>
+      <c r="C1229" s="21" t="s">
         <v>2220</v>
       </c>
       <c r="D1229" s="8" t="s">
@@ -28953,9 +29720,9 @@
       </c>
     </row>
     <row r="1230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1230" s="14"/>
-      <c r="B1230" s="14"/>
-      <c r="C1230" s="15"/>
+      <c r="A1230" s="20"/>
+      <c r="B1230" s="20"/>
+      <c r="C1230" s="21"/>
       <c r="D1230" s="6" t="s">
         <v>2222</v>
       </c>

</xml_diff>